<commit_message>
Switch to zip archives
</commit_message>
<xml_diff>
--- a/kuuube's_tablet_buying_guide.xlsx
+++ b/kuuube's_tablet_buying_guide.xlsx
@@ -32735,12 +32735,12 @@
     <mergeCell ref="K71:L71"/>
     <mergeCell ref="A72:K72"/>
     <mergeCell ref="K61:L61"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="K63:L63"/>
     <mergeCell ref="K64:L64"/>
     <mergeCell ref="K65:L65"/>
     <mergeCell ref="K66:L66"/>
     <mergeCell ref="K67:L67"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="K63:L63"/>
     <mergeCell ref="K73:L73"/>
     <mergeCell ref="K74:L74"/>
     <mergeCell ref="K75:L75"/>

</xml_diff>